<commit_message>
Actualizado Datos de Prueba Mejoras al Formulario Matriculas Mejoras al Formulario ValoresPecuniarios
</commit_message>
<xml_diff>
--- a/Datos/IED_SanPablo.xlsx
+++ b/Datos/IED_SanPablo.xlsx
@@ -13,14 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="IED_SanPablo" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9965" uniqueCount="2406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9342" uniqueCount="2406">
   <si>
     <t>ETC</t>
   </si>
@@ -42808,3134 +42807,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A623"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" t="s">
-        <v>2404</v>
-      </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339" t="s">
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" t="s">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A399" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" t="s">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A429" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" t="s">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A439" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A455" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A461" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471" t="s">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A480" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A482" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A489" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A491" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A492" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A493" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A494" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A495" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A496" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A497" t="s">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A498" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A499" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A500" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A501" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A502" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A503" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A504" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A505" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A506" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A507" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A508" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A509" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A510" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A511" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A512" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A513" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A514" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A515" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A516" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A517" t="s">
-        <v>2399</v>
-      </c>
-    </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A518" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A519" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A520" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A521" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A522" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A523" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A524" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A525" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A526" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A527" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A528" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A529" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A530" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A531" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A532" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A533" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A534" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A535" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A536" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A537" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A538" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A539" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A540" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A541" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A542" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A543" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A544" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A545" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A546" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A547" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A548" t="s">
-        <v>2396</v>
-      </c>
-    </row>
-    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A549" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A550" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A551" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A552" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A553" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A554" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A555" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A556" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A557" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A558" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A559" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A560" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A561" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A562" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A563" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="564" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A564" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A565" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="566" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A566" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="567" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A567" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="568" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A568" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="569" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A569" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="570" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A570" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="571" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A571" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="572" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A572" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="573" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A573" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="574" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A574" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="575" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A575" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A576" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="577" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A577" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="578" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A578" t="s">
-        <v>2397</v>
-      </c>
-    </row>
-    <row r="579" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A579" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="580" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A580" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="581" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A581" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="582" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A582" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="583" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A583" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="584" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A584" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="585" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A585" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="586" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A586" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="587" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A587" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="588" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A588" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="589" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A589" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="590" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A590" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="591" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A591" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="592" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A592" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="593" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A593" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="594" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A594" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="595" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A595" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="596" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A596" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="597" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A597" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="598" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A598" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="599" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A599" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A600" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="601" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A601" t="s">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A602" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="603" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A603" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="604" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A604" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="605" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A605" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="606" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A606" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="607" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A607" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="608" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A608" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="609" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A609" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="610" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A610" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="611" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A611" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="612" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A612" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="613" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A613" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="614" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A614" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="615" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A615" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="616" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A616" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="617" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A617" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="618" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A618" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="619" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A619" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="620" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A620" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="621" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A621" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="622" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A622" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-    <row r="623" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A623" t="s">
-        <v>2394</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>